<commit_message>
correcion posicion dos ultimos nodos
</commit_message>
<xml_diff>
--- a/diagrama1.xlsx
+++ b/diagrama1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enkro\Automatizacion_DiagramasDeFlujo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2C68301-950B-4A05-AD86-4824D2A0A295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACEFFB5-93E0-4A0A-AC76-6C877D1E5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5265" yWindow="2145" windowWidth="21600" windowHeight="12810" xr2:uid="{A51B9455-0DA1-4262-9C8D-5E63C3C80935}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Elemento1</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Manguera2</t>
+  </si>
+  <si>
+    <t>Manguera3</t>
+  </si>
+  <si>
+    <t>Elemento4</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,6 +489,12 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>